<commit_message>
KMR004 - Output PDF and Excel
</commit_message>
<xml_diff>
--- a/nts.uk/uk.at/at.file/nts.uk.file.at.infra/out/production/resources/report/KMR004_Template_Detail.xlsx
+++ b/nts.uk/uk.at/at.file/nts.uk.file.at.infra/out/production/resources/report/KMR004_Template_Detail.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Documents\Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anhtu\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF4B9433-02A9-43B4-9466-40A4F89C7A04}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8910"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="明細票（職場別・複数）" sheetId="2" r:id="rId1"/>
@@ -36,12 +37,11 @@
     <externalReference r:id="rId20"/>
     <externalReference r:id="rId21"/>
     <externalReference r:id="rId22"/>
-    <externalReference r:id="rId23"/>
   </externalReferences>
   <definedNames>
     <definedName name="___sss1" hidden="1">#REF!</definedName>
     <definedName name="__sss1" hidden="1">#REF!</definedName>
-    <definedName name="_ETC" hidden="1">'[2]テーブル定義書（案件番号採番）'!#REF!</definedName>
+    <definedName name="_ETC" hidden="1">'[1]テーブル定義書（案件番号採番）'!#REF!</definedName>
     <definedName name="_FFILL" hidden="1">#REF!</definedName>
     <definedName name="_Fil" hidden="1">#REF!</definedName>
     <definedName name="_Fill" localSheetId="0" hidden="1">#REF!</definedName>
@@ -69,8 +69,8 @@
     <definedName name="_面接から採用に至るまでの情報管理とする_____アウトソーシングにて_採用された情報を_ファイ__ルにて取込を行う_">#REF!</definedName>
     <definedName name="・面接から採用に至るまでの情報管理とする。___・アウトソーシングにて_採用された情報を_ファイ__ルにて取込を行う。" localSheetId="0">#REF!</definedName>
     <definedName name="・面接から採用に至るまでの情報管理とする。___・アウトソーシングにて_採用された情報を_ファイ__ルにて取込を行う。">#REF!</definedName>
-    <definedName name="a" localSheetId="0">'[3]１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ'!#REF!</definedName>
-    <definedName name="a">'[3]１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ'!#REF!</definedName>
+    <definedName name="a" localSheetId="0">'[2]１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ'!#REF!</definedName>
+    <definedName name="a">'[2]１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ'!#REF!</definedName>
     <definedName name="AA" hidden="1">#REF!</definedName>
     <definedName name="AAA" localSheetId="0">#REF!</definedName>
     <definedName name="AAA">#REF!</definedName>
@@ -88,24 +88,24 @@
     <definedName name="ｂｂｂｂ" localSheetId="0" hidden="1">{"VIEW1",#N/A,FALSE,"春木";"VIEW2",#N/A,FALSE,"春木";"VIEW3",#N/A,FALSE,"春木"}</definedName>
     <definedName name="ｂｂｂｂ" hidden="1">{"VIEW1",#N/A,FALSE,"春木";"VIEW2",#N/A,FALSE,"春木";"VIEW3",#N/A,FALSE,"春木"}</definedName>
     <definedName name="bbbbb" hidden="1">#REF!</definedName>
-    <definedName name="cal_index_size" localSheetId="0">[4]!cal_index_size</definedName>
-    <definedName name="cal_index_size">[4]!cal_index_size</definedName>
-    <definedName name="cal_table_size" localSheetId="0">[4]!cal_table_size</definedName>
-    <definedName name="cal_table_size">[4]!cal_table_size</definedName>
+    <definedName name="cal_index_size" localSheetId="0">[3]!cal_index_size</definedName>
+    <definedName name="cal_index_size">[3]!cal_index_size</definedName>
+    <definedName name="cal_table_size" localSheetId="0">[3]!cal_table_size</definedName>
+    <definedName name="cal_table_size">[3]!cal_table_size</definedName>
     <definedName name="ccc" localSheetId="0" hidden="1">{#N/A,#N/A,TRUE,"Sheet2";#N/A,#N/A,TRUE,"Sheet3";#N/A,#N/A,TRUE,"Sheet4";#N/A,#N/A,TRUE,"Sheet1"}</definedName>
     <definedName name="ccc" hidden="1">{#N/A,#N/A,TRUE,"Sheet2";#N/A,#N/A,TRUE,"Sheet3";#N/A,#N/A,TRUE,"Sheet4";#N/A,#N/A,TRUE,"Sheet1"}</definedName>
     <definedName name="ｃｃｃｃ" localSheetId="0" hidden="1">{"VIEW1",#N/A,FALSE,"懸案事項";"VIEW2",#N/A,FALSE,"懸案事項"}</definedName>
     <definedName name="ｃｃｃｃ" hidden="1">{"VIEW1",#N/A,FALSE,"懸案事項";"VIEW2",#N/A,FALSE,"懸案事項"}</definedName>
     <definedName name="ｃde" localSheetId="0" hidden="1">{"'Sheet1'!$A$1:$I$153"}</definedName>
     <definedName name="ｃde" hidden="1">{"'Sheet1'!$A$1:$I$153"}</definedName>
-    <definedName name="CULC.cal_index_size" localSheetId="0">[5]!CULC.cal_index_size</definedName>
-    <definedName name="CULC.cal_index_size">[5]!CULC.cal_index_size</definedName>
-    <definedName name="C保守単価" localSheetId="0">'[6]見積明細(ハードのみ）'!#REF!</definedName>
-    <definedName name="C保守単価">'[6]見積明細(ハードのみ）'!#REF!</definedName>
-    <definedName name="C保守委託単価" localSheetId="0">'[6]見積明細(ハードのみ）'!#REF!</definedName>
-    <definedName name="C保守委託単価">'[6]見積明細(ハードのみ）'!#REF!</definedName>
-    <definedName name="C保守支援単価" localSheetId="0">'[6]見積明細(ハードのみ）'!#REF!</definedName>
-    <definedName name="C保守支援単価">'[6]見積明細(ハードのみ）'!#REF!</definedName>
+    <definedName name="CULC.cal_index_size" localSheetId="0">[4]!CULC.cal_index_size</definedName>
+    <definedName name="CULC.cal_index_size">[4]!CULC.cal_index_size</definedName>
+    <definedName name="C保守単価" localSheetId="0">'[5]見積明細(ハードのみ）'!#REF!</definedName>
+    <definedName name="C保守単価">'[5]見積明細(ハードのみ）'!#REF!</definedName>
+    <definedName name="C保守委託単価" localSheetId="0">'[5]見積明細(ハードのみ）'!#REF!</definedName>
+    <definedName name="C保守委託単価">'[5]見積明細(ハードのみ）'!#REF!</definedName>
+    <definedName name="C保守支援単価" localSheetId="0">'[5]見積明細(ハードのみ）'!#REF!</definedName>
+    <definedName name="C保守支援単価">'[5]見積明細(ハードのみ）'!#REF!</definedName>
     <definedName name="ｄｄ" hidden="1">#REF!</definedName>
     <definedName name="ddd" localSheetId="0" hidden="1">{#N/A,#N/A,TRUE,"Sheet2";#N/A,#N/A,TRUE,"Sheet3";#N/A,#N/A,TRUE,"Sheet4";#N/A,#N/A,TRUE,"Sheet1"}</definedName>
     <definedName name="ddd" hidden="1">{#N/A,#N/A,TRUE,"Sheet2";#N/A,#N/A,TRUE,"Sheet3";#N/A,#N/A,TRUE,"Sheet4";#N/A,#N/A,TRUE,"Sheet1"}</definedName>
@@ -139,7 +139,7 @@
     <definedName name="HTML_OS" hidden="1">0</definedName>
     <definedName name="HTML_PathFile" hidden="1">"C:\My Documents\html変換\業務コード.htm"</definedName>
     <definedName name="HTML_Title" hidden="1">"業務ｺｰﾄﾞ"</definedName>
-    <definedName name="HW9707K">[7]仕切価格!$B$1:$BD$231</definedName>
+    <definedName name="HW9707K">[6]仕切価格!$B$1:$BD$231</definedName>
     <definedName name="ＩＨ" localSheetId="0">#REF!</definedName>
     <definedName name="ＩＨ">#REF!</definedName>
     <definedName name="item1" localSheetId="0">#REF!</definedName>
@@ -172,27 +172,27 @@
     <definedName name="ＭＨ">#REF!</definedName>
     <definedName name="Ｍホ" localSheetId="0">#REF!</definedName>
     <definedName name="Ｍホ">#REF!</definedName>
-    <definedName name="ｎ" localSheetId="0">'[8]１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ'!#REF!</definedName>
-    <definedName name="ｎ">'[8]１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ'!#REF!</definedName>
+    <definedName name="ｎ" localSheetId="0">'[7]１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ'!#REF!</definedName>
+    <definedName name="ｎ">'[7]１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ'!#REF!</definedName>
     <definedName name="ＯＨ" localSheetId="0">#REF!</definedName>
     <definedName name="ＯＨ">#REF!</definedName>
-    <definedName name="OPT_NO" localSheetId="0">[9]!OPT_NO</definedName>
-    <definedName name="OPT_NO">[9]!OPT_NO</definedName>
-    <definedName name="OPT_YES" localSheetId="0">[9]!OPT_YES</definedName>
-    <definedName name="OPT_YES">[9]!OPT_YES</definedName>
+    <definedName name="OPT_NO" localSheetId="0">[8]!OPT_NO</definedName>
+    <definedName name="OPT_NO">[8]!OPT_NO</definedName>
+    <definedName name="OPT_YES" localSheetId="0">[8]!OPT_YES</definedName>
+    <definedName name="OPT_YES">[8]!OPT_YES</definedName>
     <definedName name="Ｏホ" localSheetId="0">#REF!</definedName>
     <definedName name="Ｏホ">#REF!</definedName>
-    <definedName name="PG単価" localSheetId="0">[10]明細合計!#REF!</definedName>
-    <definedName name="PG単価">[10]明細合計!#REF!</definedName>
+    <definedName name="PG単価" localSheetId="0">[9]明細合計!#REF!</definedName>
+    <definedName name="PG単価">[9]明細合計!#REF!</definedName>
     <definedName name="PG田中" localSheetId="0">#REF!</definedName>
     <definedName name="PG田中">#REF!</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'明細票（職場別・複数）'!$A$1:$L$11</definedName>
-    <definedName name="PrintDaicho" localSheetId="0">[11]!PrintDaicho</definedName>
-    <definedName name="PrintDaicho">[11]!PrintDaicho</definedName>
-    <definedName name="QuitDaicho" localSheetId="0">[11]!QuitDaicho</definedName>
-    <definedName name="QuitDaicho">[11]!QuitDaicho</definedName>
-    <definedName name="SE単価" localSheetId="0">[10]明細合計!#REF!</definedName>
-    <definedName name="SE単価">[10]明細合計!#REF!</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'明細票（職場別・複数）'!#REF!</definedName>
+    <definedName name="PrintDaicho" localSheetId="0">[10]!PrintDaicho</definedName>
+    <definedName name="PrintDaicho">[10]!PrintDaicho</definedName>
+    <definedName name="QuitDaicho" localSheetId="0">[10]!QuitDaicho</definedName>
+    <definedName name="QuitDaicho">[10]!QuitDaicho</definedName>
+    <definedName name="SE単価" localSheetId="0">[9]明細合計!#REF!</definedName>
+    <definedName name="SE単価">[9]明細合計!#REF!</definedName>
     <definedName name="sisann" hidden="1">#REF!</definedName>
     <definedName name="sss" localSheetId="0" hidden="1">#REF!</definedName>
     <definedName name="sss" hidden="1">#REF!</definedName>
@@ -203,9 +203,9 @@
     <definedName name="ＳＷ" localSheetId="0">#REF!</definedName>
     <definedName name="ＳＷ">#REF!</definedName>
     <definedName name="Ver002001006特休残管理対応" hidden="1">#REF!</definedName>
-    <definedName name="ｗ" localSheetId="0">'[6]見積明細(ハードのみ）'!#REF!</definedName>
-    <definedName name="ｗ">'[6]見積明細(ハードのみ）'!#REF!</definedName>
-    <definedName name="WC単価">'[6]見積明細(ハードのみ）'!$X$5:$X$34</definedName>
+    <definedName name="ｗ" localSheetId="0">'[5]見積明細(ハードのみ）'!#REF!</definedName>
+    <definedName name="ｗ">'[5]見積明細(ハードのみ）'!#REF!</definedName>
+    <definedName name="WC単価">'[5]見積明細(ハードのみ）'!$X$5:$X$34</definedName>
     <definedName name="wrn.MIND." localSheetId="0" hidden="1">{#N/A,#N/A,TRUE,"Sheet2";#N/A,#N/A,TRUE,"Sheet3";#N/A,#N/A,TRUE,"Sheet4";#N/A,#N/A,TRUE,"Sheet1"}</definedName>
     <definedName name="wrn.MIND." hidden="1">{#N/A,#N/A,TRUE,"Sheet2";#N/A,#N/A,TRUE,"Sheet3";#N/A,#N/A,TRUE,"Sheet4";#N/A,#N/A,TRUE,"Sheet1"}</definedName>
     <definedName name="wrn.PRINT_ALL." localSheetId="0" hidden="1">{"VIEW1",#N/A,FALSE,"春木";"VIEW2",#N/A,FALSE,"春木";"VIEW3",#N/A,FALSE,"春木"}</definedName>
@@ -231,8 +231,8 @@
     <definedName name="い" localSheetId="0" hidden="1">#REF!</definedName>
     <definedName name="い" hidden="1">#REF!</definedName>
     <definedName name="え" hidden="1">#REF!</definedName>
-    <definedName name="えらー" hidden="1">[12]表紙!#REF!</definedName>
-    <definedName name="エラー一覧" hidden="1">[12]表紙!#REF!</definedName>
+    <definedName name="えらー" hidden="1">[11]表紙!#REF!</definedName>
+    <definedName name="エラー一覧" hidden="1">[11]表紙!#REF!</definedName>
     <definedName name="クＨ" localSheetId="0">#REF!</definedName>
     <definedName name="クＨ">#REF!</definedName>
     <definedName name="クサＨ" localSheetId="0">#REF!</definedName>
@@ -245,17 +245,17 @@
     <definedName name="クニホ">#REF!</definedName>
     <definedName name="クホ" localSheetId="0">#REF!</definedName>
     <definedName name="クホ">#REF!</definedName>
-    <definedName name="サＨ" localSheetId="0">'[13]１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ'!#REF!</definedName>
-    <definedName name="サＨ">'[13]１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ'!#REF!</definedName>
-    <definedName name="サホ" localSheetId="0">'[13]１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ'!#REF!</definedName>
-    <definedName name="サホ">'[13]１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ'!#REF!</definedName>
+    <definedName name="サＨ" localSheetId="0">'[12]１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ'!#REF!</definedName>
+    <definedName name="サＨ">'[12]１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ'!#REF!</definedName>
+    <definedName name="サホ" localSheetId="0">'[12]１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ'!#REF!</definedName>
+    <definedName name="サホ">'[12]１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ'!#REF!</definedName>
     <definedName name="サホ1" localSheetId="0">#REF!</definedName>
     <definedName name="サホ1">#REF!</definedName>
     <definedName name="ｻﾎﾟｰﾄﾏﾆｭｱﾙ" hidden="1">#REF!</definedName>
     <definedName name="サンプル" hidden="1">#REF!</definedName>
-    <definedName name="サンプル２" hidden="1">[12]表紙!#REF!</definedName>
-    <definedName name="サンプルあ" hidden="1">[12]表紙!#REF!</definedName>
-    <definedName name="すすす" hidden="1">[12]定義書!#REF!</definedName>
+    <definedName name="サンプル２" hidden="1">[11]表紙!#REF!</definedName>
+    <definedName name="サンプルあ" hidden="1">[11]表紙!#REF!</definedName>
+    <definedName name="すすす" hidden="1">[11]定義書!#REF!</definedName>
     <definedName name="だ" localSheetId="0" hidden="1">{"'Sheet1'!$A$1:$I$153"}</definedName>
     <definedName name="だ" hidden="1">{"'Sheet1'!$A$1:$I$153"}</definedName>
     <definedName name="タスクドキュメント１" hidden="1">#REF!</definedName>
@@ -263,8 +263,8 @@
     <definedName name="ｯb" hidden="1">{"'Sheet1'!$A$1:$I$153"}</definedName>
     <definedName name="ツール別見積工数" localSheetId="0">#REF!</definedName>
     <definedName name="ツール別見積工数">#REF!</definedName>
-    <definedName name="ディテール" hidden="1">[12]表紙!#REF!</definedName>
-    <definedName name="テーブル項目">[14]項目定義書!$A$3:$E$364</definedName>
+    <definedName name="ディテール" hidden="1">[11]表紙!#REF!</definedName>
+    <definedName name="テーブル項目">[13]項目定義書!$A$3:$E$364</definedName>
     <definedName name="テスト５" localSheetId="0" hidden="1">{"'Sheet1'!$A$1:$I$153"}</definedName>
     <definedName name="テスト５" hidden="1">{"'Sheet1'!$A$1:$I$153"}</definedName>
     <definedName name="てててて" localSheetId="0" hidden="1">{"'Sheet1'!$A$1:$I$153"}</definedName>
@@ -292,46 +292,46 @@
     <definedName name="ヘッダー" localSheetId="0">#REF!</definedName>
     <definedName name="ヘッダー">#REF!</definedName>
     <definedName name="ボタン制御マトリクス" hidden="1">#REF!</definedName>
-    <definedName name="ユーザー一覧" localSheetId="0">'[15]工数計算(ﾈｯﾄﾜｰｸ）'!#REF!</definedName>
-    <definedName name="ユーザー一覧">'[15]工数計算(ﾈｯﾄﾜｰｸ）'!#REF!</definedName>
-    <definedName name="ワイドに" localSheetId="0">[16]!ワイドに</definedName>
-    <definedName name="ワイドに">[16]!ワイドに</definedName>
+    <definedName name="ユーザー一覧" localSheetId="0">'[14]工数計算(ﾈｯﾄﾜｰｸ）'!#REF!</definedName>
+    <definedName name="ユーザー一覧">'[14]工数計算(ﾈｯﾄﾜｰｸ）'!#REF!</definedName>
+    <definedName name="ワイドに" localSheetId="0">[15]!ワイドに</definedName>
+    <definedName name="ワイドに">[15]!ワイドに</definedName>
     <definedName name="んんんん" localSheetId="0" hidden="1">{"'Sheet1'!$A$1:$I$153"}</definedName>
     <definedName name="んんんん" hidden="1">{"'Sheet1'!$A$1:$I$153"}</definedName>
     <definedName name="一般社員時間外労働手当部門別集計ｸｴﾘｰ" localSheetId="0">#REF!</definedName>
     <definedName name="一般社員時間外労働手当部門別集計ｸｴﾘｰ">#REF!</definedName>
     <definedName name="人日原価" localSheetId="0">#REF!</definedName>
     <definedName name="人日原価">#REF!</definedName>
-    <definedName name="仕切り">'[6]見積明細(ハードのみ）'!$R$5:$R$34</definedName>
-    <definedName name="仕切単価">'[6]見積明細(ハードのみ）'!$R$5:$R$34</definedName>
+    <definedName name="仕切り">'[5]見積明細(ハードのみ）'!$R$5:$R$34</definedName>
+    <definedName name="仕切単価">'[5]見積明細(ハードのみ）'!$R$5:$R$34</definedName>
     <definedName name="住民税115" localSheetId="0">#REF!</definedName>
     <definedName name="住民税115">#REF!</definedName>
     <definedName name="住民税96">#REF!</definedName>
     <definedName name="住民税納付先の登録7">#REF!</definedName>
     <definedName name="価格表" localSheetId="0">#REF!</definedName>
     <definedName name="価格表">#REF!</definedName>
-    <definedName name="保守単価">'[6]見積明細(ハードのみ）'!$L$5:$L$34</definedName>
-    <definedName name="保守委託単価">'[6]見積明細(ハードのみ）'!$N$5:$N$34</definedName>
-    <definedName name="保守支援単価">'[6]見積明細(ハードのみ）'!$P$5:$P$34</definedName>
-    <definedName name="値引単価">'[6]見積明細(ハードのみ）'!$J$5:$J$34</definedName>
-    <definedName name="備考">'[6]見積明細(ハードのみ）'!$AA$5:$AA$34</definedName>
+    <definedName name="保守単価">'[5]見積明細(ハードのみ）'!$L$5:$L$34</definedName>
+    <definedName name="保守委託単価">'[5]見積明細(ハードのみ）'!$N$5:$N$34</definedName>
+    <definedName name="保守支援単価">'[5]見積明細(ハードのみ）'!$P$5:$P$34</definedName>
+    <definedName name="値引単価">'[5]見積明細(ハードのみ）'!$J$5:$J$34</definedName>
+    <definedName name="備考">'[5]見積明細(ハードのみ）'!$AA$5:$AA$34</definedName>
     <definedName name="処理サイクル" localSheetId="0" hidden="1">{"'Sheet1'!$A$1:$I$153"}</definedName>
     <definedName name="処理サイクル" hidden="1">{"'Sheet1'!$A$1:$I$153"}</definedName>
-    <definedName name="削除０１" hidden="1">'[2]テーブル定義書（案件番号採番）'!#REF!</definedName>
+    <definedName name="削除０１" hidden="1">'[1]テーブル定義書（案件番号採番）'!#REF!</definedName>
     <definedName name="削除０２" hidden="1">#REF!</definedName>
     <definedName name="削除０３" hidden="1">#REF!</definedName>
-    <definedName name="削除０４" hidden="1">'[2]テーブル定義書（案件番号採番）'!#REF!</definedName>
+    <definedName name="削除０４" hidden="1">'[1]テーブル定義書（案件番号採番）'!#REF!</definedName>
     <definedName name="削除０５" hidden="1">#REF!</definedName>
     <definedName name="削除０６" hidden="1">#REF!</definedName>
-    <definedName name="削除０７" hidden="1">'[2]テーブル定義書（案件番号採番）'!#REF!</definedName>
+    <definedName name="削除０７" hidden="1">'[1]テーブル定義書（案件番号採番）'!#REF!</definedName>
     <definedName name="削除０８" hidden="1">#REF!</definedName>
     <definedName name="削除０９" hidden="1">#REF!</definedName>
     <definedName name="単価" localSheetId="0">#REF!</definedName>
     <definedName name="単価">#REF!</definedName>
     <definedName name="単価種別" localSheetId="0">#REF!</definedName>
     <definedName name="単価種別">#REF!</definedName>
-    <definedName name="印刷" localSheetId="0">[17]!印刷</definedName>
-    <definedName name="印刷">[17]!印刷</definedName>
+    <definedName name="印刷" localSheetId="0">[16]!印刷</definedName>
+    <definedName name="印刷">[16]!印刷</definedName>
     <definedName name="原価" localSheetId="0">#REF!</definedName>
     <definedName name="原価">#REF!</definedName>
     <definedName name="売値" localSheetId="0">#REF!</definedName>
@@ -350,9 +350,9 @@
     <definedName name="日帰り単金">#REF!</definedName>
     <definedName name="概要_基準日設定" localSheetId="0" hidden="1">#REF!</definedName>
     <definedName name="概要_基準日設定" hidden="1">#REF!</definedName>
-    <definedName name="標準価格">'[6]見積明細(ハードのみ）'!$C$5:$H$34</definedName>
-    <definedName name="機種SORT" localSheetId="0">[18]!機種SORT</definedName>
-    <definedName name="機種SORT">[19]!機種SORT</definedName>
+    <definedName name="標準価格">'[5]見積明細(ハードのみ）'!$C$5:$H$34</definedName>
+    <definedName name="機種SORT" localSheetId="0">[17]!機種SORT</definedName>
+    <definedName name="機種SORT">[18]!機種SORT</definedName>
     <definedName name="機能別原価" localSheetId="0">#REF!</definedName>
     <definedName name="機能別原価">#REF!</definedName>
     <definedName name="画面1">#REF!</definedName>
@@ -362,14 +362,14 @@
     <definedName name="画面5">#REF!</definedName>
     <definedName name="画面6">#REF!</definedName>
     <definedName name="画面7">#REF!</definedName>
-    <definedName name="直扱単価">'[6]見積明細(ハードのみ）'!$V$5:$V$34</definedName>
-    <definedName name="社共単価">'[6]見積明細(ハードのみ）'!$T$5:$T$34</definedName>
+    <definedName name="直扱単価">'[5]見積明細(ハードのみ）'!$V$5:$V$34</definedName>
+    <definedName name="社共単価">'[5]見積明細(ハードのみ）'!$T$5:$T$34</definedName>
     <definedName name="種別" localSheetId="0">#REF!</definedName>
     <definedName name="種別">#REF!</definedName>
-    <definedName name="終了" localSheetId="0">[20]!終了</definedName>
-    <definedName name="終了">[20]!終了</definedName>
-    <definedName name="見やすく" localSheetId="0">[16]!見やすく</definedName>
-    <definedName name="見やすく">[16]!見やすく</definedName>
+    <definedName name="終了" localSheetId="0">[19]!終了</definedName>
+    <definedName name="終了">[19]!終了</definedName>
+    <definedName name="見やすく" localSheetId="0">[15]!見やすく</definedName>
+    <definedName name="見やすく">[15]!見やすく</definedName>
     <definedName name="見積工数" localSheetId="0">#REF!</definedName>
     <definedName name="見積工数">#REF!</definedName>
     <definedName name="解析">#N/A</definedName>
@@ -378,16 +378,16 @@
     <definedName name="返戻種類追加" hidden="1">{"'Sheet1'!$A$1:$I$153"}</definedName>
     <definedName name="返戻種類追加２" localSheetId="0" hidden="1">{"'Sheet1'!$A$1:$I$153"}</definedName>
     <definedName name="返戻種類追加２" hidden="1">{"'Sheet1'!$A$1:$I$153"}</definedName>
-    <definedName name="部">'[6]見積明細(ハードのみ）'!$Z$5:$Z$34</definedName>
+    <definedName name="部">'[5]見積明細(ハードのみ）'!$Z$5:$Z$34</definedName>
     <definedName name="部門別時間外労働手当状況" localSheetId="0">#REF!</definedName>
     <definedName name="部門別時間外労働手当状況">#REF!</definedName>
-    <definedName name="重複" hidden="1">[21]表紙!#REF!</definedName>
+    <definedName name="重複" hidden="1">[20]表紙!#REF!</definedName>
     <definedName name="銀行の登録48">#REF!</definedName>
     <definedName name="銀行の登録67">#REF!</definedName>
     <definedName name="銀行の登録7">#REF!</definedName>
     <definedName name="関連表" hidden="1">#REF!</definedName>
     <definedName name="関連表２" hidden="1">#REF!</definedName>
-    <definedName name="電子帳票仕様" hidden="1">[22]表紙!#REF!</definedName>
+    <definedName name="電子帳票仕様" hidden="1">[21]表紙!#REF!</definedName>
     <definedName name="電車" localSheetId="0">#REF!</definedName>
     <definedName name="電車">#REF!</definedName>
     <definedName name="項目名の登録1" localSheetId="0">#REF!</definedName>
@@ -419,61 +419,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="8">
-  <si>
-    <t>社員コード</t>
-    <rPh sb="0" eb="2">
-      <t>シャイン</t>
-    </rPh>
-    <phoneticPr fontId="0"/>
-  </si>
-  <si>
-    <t>社員名</t>
-    <rPh sb="0" eb="2">
-      <t>シャイン</t>
-    </rPh>
-    <rPh sb="2" eb="3">
-      <t>メイ</t>
-    </rPh>
-    <phoneticPr fontId="0"/>
-  </si>
-  <si>
-    <t>数量</t>
-    <rPh sb="0" eb="2">
-      <t>スウリョウ</t>
-    </rPh>
-    <phoneticPr fontId="0"/>
-  </si>
-  <si>
-    <t>チェック</t>
-    <phoneticPr fontId="0"/>
-  </si>
-  <si>
-    <t>合計</t>
-    <rPh sb="0" eb="2">
-      <t>ゴウケイ</t>
-    </rPh>
-    <phoneticPr fontId="0"/>
-  </si>
-  <si>
-    <t>個</t>
-    <rPh sb="0" eb="1">
-      <t>コ</t>
-    </rPh>
-    <phoneticPr fontId="0"/>
-  </si>
-  <si>
-    <t>職場○：</t>
-  </si>
-  <si>
-    <t>　期間：</t>
-  </si>
-</sst>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -489,290 +440,27 @@
       <charset val="128"/>
     </font>
     <font>
-      <sz val="7"/>
-      <color theme="1"/>
-      <name val="ＭＳ ゴシック"/>
-      <family val="3"/>
-      <charset val="128"/>
-    </font>
-    <font>
       <sz val="9"/>
       <color theme="1"/>
       <name val="ＭＳ ゴシック"/>
       <family val="3"/>
       <charset val="128"/>
     </font>
-    <font>
-      <sz val="7"/>
-      <name val="ＭＳ ゴシック"/>
-      <family val="3"/>
-      <charset val="128"/>
-    </font>
-    <font>
-      <sz val="7"/>
-      <color theme="1"/>
-      <name val="源ノ角ゴシック Normal"/>
-      <family val="2"/>
-      <charset val="128"/>
-    </font>
   </fonts>
-  <fills count="5">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFDDEBF7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="20">
+  <borders count="1">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="dotted">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="dotted">
-        <color indexed="64"/>
-      </left>
-      <right style="dotted">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="dotted">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="dotted">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="dotted">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="dotted">
-        <color indexed="64"/>
-      </left>
-      <right style="dotted">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="dotted">
-        <color indexed="64"/>
-      </left>
-      <right style="dotted">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="dotted">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="dotted">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="dotted">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="dotted">
-        <color indexed="64"/>
-      </left>
-      <right style="dotted">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="dotted">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="dotted">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="double">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="double">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -782,109 +470,15 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="13" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="標準 3" xfId="1"/>
+    <cellStyle name="標準 3" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -903,39 +497,18 @@
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
-      <sheetName val="明細票（職場別・複数）"/>
-      <sheetName val="明細票（職場別・最大行）"/>
-      <sheetName val="明細票（職場別・改行)"/>
-      <sheetName val="明細票（場所別・複数） "/>
-      <sheetName val="明細票（場所別・最大行）"/>
-      <sheetName val="明細票（場所別・改行)"/>
+      <sheetName val="テーブル定義書（案件番号採番）"/>
+      <sheetName val="案件採番ﾃｰﾌﾞﾙ"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
+      <sheetData sheetId="1" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
 </file>
 
 <file path=xl/externalLinks/externalLink10.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="明細合計"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink11.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
@@ -958,7 +531,7 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink11.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
@@ -1017,7 +590,7 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink12.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
@@ -1030,7 +603,7 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink13.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
@@ -6326,7 +5899,7 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink14.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
@@ -6359,7 +5932,7 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink15.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
@@ -6508,7 +6081,7 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink16.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
@@ -6519,6 +6092,24 @@
     </definedNames>
     <sheetDataSet>
       <sheetData sheetId="0" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink17.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="画面イメージ(振込一覧表） (2)"/>
+      <sheetName val="アコーディオン画面"/>
+    </sheetNames>
+    <definedNames>
+      <definedName name="機種SORT" refersTo="#REF!"/>
+    </definedNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -6546,39 +6137,6 @@
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
-      <sheetName val="画面イメージ(振込一覧表） (2)"/>
-      <sheetName val="アコーディオン画面"/>
-    </sheetNames>
-    <definedNames>
-      <definedName name="機種SORT" refersTo="#REF!"/>
-    </definedNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="テーブル定義書（案件番号採番）"/>
-      <sheetName val="案件採番ﾃｰﾌﾞﾙ"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink20.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
       <sheetName val="COPYFAN"/>
     </sheetNames>
     <definedNames>
@@ -6591,7 +6149,24 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ"/>
+      <sheetName val="master"/>
+      <sheetName val="Sheet1"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="2" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink20.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
@@ -6618,7 +6193,7 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink21.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
@@ -6655,23 +6230,6 @@
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
-      <sheetName val="１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ"/>
-      <sheetName val="master"/>
-      <sheetName val="Sheet1"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink4.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
       <sheetName val="見積支援"/>
       <sheetName val="Sheet1"/>
       <sheetName val="業務（自動）_NET"/>
@@ -6691,7 +6249,7 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink4.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
@@ -6773,7 +6331,7 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink5.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
@@ -8257,7 +7815,7 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink6.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
@@ -44619,7 +44177,7 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink7.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
@@ -44632,7 +44190,7 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink8.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
@@ -44646,6 +44204,19 @@
     <sheetDataSet>
       <sheetData sheetId="0" refreshError="1"/>
       <sheetData sheetId="1" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink9.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="明細合計"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -44913,177 +44484,33 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor theme="9" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:L9"/>
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="2.7109375" defaultRowHeight="11.25"/>
+  <sheetFormatPr defaultColWidth="2.6640625" defaultRowHeight="10.8"/>
   <cols>
-    <col min="1" max="1" width="9.5703125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="11.140625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="3.42578125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="7.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.42578125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="11.42578125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="3.42578125" style="2" customWidth="1"/>
-    <col min="8" max="8" width="7.28515625" style="2" customWidth="1"/>
-    <col min="9" max="9" width="9.5703125" style="2" customWidth="1"/>
-    <col min="10" max="10" width="11.42578125" style="2" customWidth="1"/>
-    <col min="11" max="11" width="3.42578125" style="2" customWidth="1"/>
-    <col min="12" max="12" width="7.28515625" style="2" customWidth="1"/>
-    <col min="13" max="16384" width="2.7109375" style="2"/>
+    <col min="1" max="1" width="9.5546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="11.109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="3.44140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="7.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.44140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="11.44140625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="3.44140625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="7.33203125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="9.5546875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="11.44140625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="3.44140625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="7.33203125" style="1" customWidth="1"/>
+    <col min="13" max="16384" width="2.6640625" style="1"/>
   </cols>
-  <sheetData>
-    <row r="1" spans="1:12">
-      <c r="A1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" s="3"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-    </row>
-    <row r="2" spans="1:12">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-    </row>
-    <row r="3" spans="1:12" ht="12" thickBot="1">
-      <c r="A3" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="7"/>
-      <c r="J3" s="7"/>
-      <c r="K3" s="7"/>
-      <c r="L3" s="7"/>
-    </row>
-    <row r="4" spans="1:12">
-      <c r="A4" s="8"/>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8"/>
-      <c r="I4" s="9"/>
-      <c r="J4" s="8"/>
-      <c r="K4" s="8"/>
-      <c r="L4" s="8"/>
-    </row>
-    <row r="5" spans="1:12" ht="12" thickBot="1">
-      <c r="A5" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="D5" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="E5" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="F5" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="G5" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="H5" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="I5" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="J5" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="K5" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="L5" s="15" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12">
-      <c r="A6" s="16"/>
-      <c r="B6" s="17"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="19"/>
-      <c r="E6" s="20"/>
-      <c r="F6" s="17"/>
-      <c r="G6" s="18"/>
-      <c r="H6" s="19"/>
-      <c r="I6" s="20"/>
-      <c r="J6" s="17"/>
-      <c r="K6" s="18"/>
-      <c r="L6" s="21"/>
-    </row>
-    <row r="7" spans="1:12" ht="12" thickBot="1">
-      <c r="A7" s="22"/>
-      <c r="B7" s="23"/>
-      <c r="C7" s="23"/>
-      <c r="D7" s="24"/>
-      <c r="E7" s="25"/>
-      <c r="F7" s="23"/>
-      <c r="G7" s="23"/>
-      <c r="H7" s="24"/>
-      <c r="I7" s="25"/>
-      <c r="J7" s="23"/>
-      <c r="K7" s="23"/>
-      <c r="L7" s="26"/>
-    </row>
-    <row r="8" spans="1:12" ht="12" thickTop="1">
-      <c r="A8" s="27"/>
-      <c r="B8" s="27"/>
-      <c r="C8" s="27"/>
-      <c r="D8" s="27"/>
-      <c r="E8" s="28"/>
-      <c r="F8" s="28"/>
-      <c r="G8" s="27"/>
-      <c r="H8" s="29"/>
-      <c r="I8" s="27"/>
-      <c r="J8" s="27" t="s">
-        <v>4</v>
-      </c>
-      <c r="K8" s="27"/>
-      <c r="L8" s="29" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" ht="12" thickBot="1">
-      <c r="A9" s="30"/>
-      <c r="B9" s="31"/>
-      <c r="C9" s="31"/>
-      <c r="D9" s="31"/>
-      <c r="E9" s="32"/>
-      <c r="F9" s="31"/>
-      <c r="G9" s="31"/>
-      <c r="H9" s="31"/>
-      <c r="I9" s="33"/>
-      <c r="J9" s="33"/>
-      <c r="K9" s="33"/>
-      <c r="L9" s="33"/>
-    </row>
-  </sheetData>
+  <sheetData/>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.98425196850393704" bottom="0.39370078740157483" header="0.39370078740157483" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>